<commit_message>
fix excel content and link
</commit_message>
<xml_diff>
--- a/bakrang/excel/template/school.xlsx
+++ b/bakrang/excel/template/school.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szymon Sobiepanek\sobies93.github.io\bakrang\excel\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E94371A-7873-473C-8057-8EDAFAC200FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBA90F6-3E59-44A7-81B7-6312F2955404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{FE612A00-576E-43D6-B712-5E98FA4A6106}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FE612A00-576E-43D6-B712-5E98FA4A6106}"/>
   </bookViews>
   <sheets>
     <sheet name="Number of students" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E698E08-5D3E-4D2D-9D94-8C8119EAE53C}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
@@ -750,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082FC4B1-C252-49FE-8EDE-63ABB42A0043}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change label description in excel
</commit_message>
<xml_diff>
--- a/bakrang/excel/template/school.xlsx
+++ b/bakrang/excel/template/school.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szymon Sobiepanek\sobies93.github.io\bakrang\excel\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBA90F6-3E59-44A7-81B7-6312F2955404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5008CA20-93F5-41F2-AFF7-2B532713DF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FE612A00-576E-43D6-B712-5E98FA4A6106}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Total</t>
   </si>
@@ -118,6 +118,36 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>class 1</t>
+  </si>
+  <si>
+    <t>class 2</t>
+  </si>
+  <si>
+    <t>class 3</t>
+  </si>
+  <si>
+    <t>class 4</t>
+  </si>
+  <si>
+    <t>class 5</t>
+  </si>
+  <si>
+    <t>class 6</t>
+  </si>
+  <si>
+    <t>class 7</t>
+  </si>
+  <si>
+    <t>class 8</t>
+  </si>
+  <si>
+    <t>class 9</t>
+  </si>
+  <si>
+    <t>class 10</t>
   </si>
 </sst>
 </file>
@@ -191,9 +221,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -231,7 +261,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -337,7 +367,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -479,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -490,41 +520,41 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>0</v>
@@ -741,6 +771,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>